<commit_message>
COMMIT UPDATE GEN PDF
</commit_message>
<xml_diff>
--- a/Attestati Corsi di Formazione/report_gen_data/db/db_corsi.xlsx
+++ b/Attestati Corsi di Formazione/report_gen_data/db/db_corsi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">odoo_id</t>
   </si>
@@ -56,6 +56,23 @@
   </si>
   <si>
     <t xml:space="preserve">Responsabilità d'Impresa: Il D.Lgs. 231/2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La normativa del D.Lgs 231/2001 principi generali  
+a cura del Presidente OdV Prof. Paolo Fratini 
+Il sistema sanzionatorio ed elenco dei reati presupposto  
+a cura del Membro OdV Fabio Calaciura 
+I reati fiscali e societari nella normativa 231 
+a cura del Membro OdV Dott. Marco Rosatelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modello 231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nozioni di sicurezza alimentare e applicazione HACCP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacchetto Igiene</t>
   </si>
   <si>
     <t xml:space="preserve">TESTO DA RIEMPIRE - TESTO DA RIEMPIRE
@@ -64,15 +81,6 @@
 testo da riempire con i contenuti del corso - testo da riempire con i contenuti del corso - 
 testo da riempire con i contenuti del corso - testo da riempire con i contenuti del corso - 
 testo da riempire con i contenuti del corso - testo da riempire con i contenuti del corso - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modello 231</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nozioni di sicurezza alimentare e applicazione HACCP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pacchetto Igiene</t>
   </si>
   <si>
     <t xml:space="preserve">HACCP e Celiachia</t>
@@ -159,20 +167,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -371,84 +383,84 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="27.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="n">
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MAIN UPDATE working version
</commit_message>
<xml_diff>
--- a/Attestati Corsi di Formazione/report_gen_data/db/db_corsi.xlsx
+++ b/Attestati Corsi di Formazione/report_gen_data/db/db_corsi.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="db_corsi" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="db_corsi" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,43 +21,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t xml:space="preserve">odoo_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nome_corso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contenuti_corso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">durata_corso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CORSO SICUREZZA SUL LAVORO 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salute e Sicurezza nei Luoghi di Lavoro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FORMAZIONE GENERALE: Normativa di riferimento . Concetti di Rischio, Danno, Prevenzione e Protezione. Organizzazione della prevenzione aziendale; Diritti, doveri e sanzioni per i vari soggetti aziendali; Organi di vigilanza, controllo e assistenza. 
+    <t>odoo_id</t>
+  </si>
+  <si>
+    <t>nome_corso</t>
+  </si>
+  <si>
+    <t>contenuti_corso</t>
+  </si>
+  <si>
+    <t>durata_corso</t>
+  </si>
+  <si>
+    <t>save_path</t>
+  </si>
+  <si>
+    <t>CORSO SICUREZZA SUL LAVORO 2025</t>
+  </si>
+  <si>
+    <t>Salute e Sicurezza nei Luoghi di Lavoro</t>
+  </si>
+  <si>
+    <t>FORMAZIONE GENERALE: Normativa di riferimento . Concetti di Rischio, Danno, Prevenzione e Protezione. Organizzazione della prevenzione aziendale; Diritti, doveri e sanzioni per i vari soggetti aziendali; Organi di vigilanza, controllo e assistenza. 
 FORMAZIONE RISCHIO SPECIFICO _ BASSO : Rischi infortuni; Meccanici generali; Elettrici generali; Macchine; Attrezzature; Rischi chimici; Nebbie Oli Fumi Vapori 
 Polveri: Etichettatura; ; Rischi biologici, Analisi del rischio di diffusione del Coronavirus e misure per il contenimento; Rischi fisici; Rumore; Vibrazione; Radiazioni; Microclima e illuminazione; Videoterminali; DPI Organizzazione del lavoro; Ambienti di lavoro; Stress lavoro correlato; Movimentazione manuale carichi; Movimentazione manuale carichi; Segnaletica; Emergenze; 
  Le procedure di sicurezza con riferimento al profilo di rischio del comparto di riferimento al codice ATECO e al Profilo professionale; Procedure esodo e incendi; Procedure organizzative per il primo soccorso; Incidenti e infortuni mancati; Altri Rischi. Test di verifica finale</t>
   </si>
   <si>
-    <t xml:space="preserve">Sicurezza sul Lavoro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FORMAZIONE 231</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Responsabilità d'Impresa: Il D.Lgs. 231/2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La normativa del D.Lgs 231/2001 principi generali  
+    <t>Sicurezza sul Lavoro</t>
+  </si>
+  <si>
+    <t>FORMAZIONE 231</t>
+  </si>
+  <si>
+    <t>Responsabilità d'Impresa: Il D.Lgs. 231/2001</t>
+  </si>
+  <si>
+    <t>La normativa del D.Lgs 231/2001 principi generali  
 a cura del Presidente OdV Prof. Paolo Fratini 
 Il sistema sanzionatorio ed elenco dei reati presupposto  
 a cura del Membro OdV Fabio Calaciura 
@@ -66,13 +65,13 @@
 a cura del Membro OdV Dott. Marco Rosatelli</t>
   </si>
   <si>
-    <t xml:space="preserve">Modello 231</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nozioni di sicurezza alimentare e applicazione HACCP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pacchetto Igiene</t>
+    <t>Modello 231</t>
+  </si>
+  <si>
+    <t>Nozioni di sicurezza alimentare e applicazione HACCP</t>
+  </si>
+  <si>
+    <t>Pacchetto Igiene</t>
   </si>
   <si>
     <t xml:space="preserve">TESTO DA RIEMPIRE - TESTO DA RIEMPIRE
@@ -83,17 +82,14 @@
 testo da riempire con i contenuti del corso - testo da riempire con i contenuti del corso - </t>
   </si>
   <si>
-    <t xml:space="preserve">HACCP e Celiachia</t>
+    <t>HACCP e Celiachia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,22 +98,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -134,7 +115,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -142,100 +123,67 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -243,12 +191,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -277,7 +225,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -298,7 +246,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -349,7 +297,7 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -367,35 +315,34 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="27.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.71"/>
+    <col min="1" max="1" width="49.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -412,7 +359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -422,14 +369,14 @@
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -439,14 +386,14 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -456,7 +403,7 @@
       <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="4">
         <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -464,12 +411,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update template PDF corso anticorruzione
</commit_message>
<xml_diff>
--- a/Attestati Corsi di Formazione/report_gen_data/db/db_corsi.xlsx
+++ b/Attestati Corsi di Formazione/report_gen_data/db/db_corsi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t xml:space="preserve">odoo_id</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t xml:space="preserve">HACCP e Celiachia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORSO IN MATERIA DI PREVENZIONE DELLA CORRUZIONE E DELL'ILLEGALITA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definizioni operative del fenomeno corruttivo , Quadro normativo: art. 318 c.p. e art. 2635 c.c., Tipologie di corruzione: propria, impropria, ambientale e tra privati, Pene e circostanze aggravanti, Responsabilità individuali e aziendali, Policy interna anti-corruzione: obiettivi e ambito di applicazione, Procedure di segnalazione interna ed esterna, con garanzia di anonimato, Best practice etiche e strategie di compliance per il contrasto della corruzione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti Corruzione</t>
   </si>
 </sst>
 </file>
@@ -88,7 +97,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +133,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,7 +184,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -191,6 +207,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -385,10 +405,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -468,6 +488,23 @@
         <v>16</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="32.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>